<commit_message>
new links for examples
</commit_message>
<xml_diff>
--- a/content/input/summary-opendata.xlsx
+++ b/content/input/summary-opendata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina Andrade\Documents\GitHub\coes\lisa-coes\content\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C85C908-B1CB-417C-84B6-95D76B9F8463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E2997E-7F4E-4BEF-8C89-9B82DF36F0C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3310" yWindow="1830" windowWidth="14400" windowHeight="7370" xr2:uid="{04B4ED3C-72C1-4A08-99FB-78FDB9FB65F1}"/>
+    <workbookView xWindow="7170" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{04B4ED3C-72C1-4A08-99FB-78FDB9FB65F1}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
   <si>
     <t>Elemento</t>
   </si>
@@ -133,16 +133,28 @@
     <t>Ejemplo 4</t>
   </si>
   <si>
-    <t>Ejemplo de base de datos</t>
-  </si>
-  <si>
-    <t>Ejemplo de cuestionario</t>
-  </si>
-  <si>
-    <t>Ejemplo de libro de códigos</t>
-  </si>
-  <si>
-    <t>Ejemplo de ficha técnica</t>
+    <t>1. 1 Ejemplo de base de datos</t>
+  </si>
+  <si>
+    <t>1.2 Ejemplo de base de datos</t>
+  </si>
+  <si>
+    <t>1.1 Ejemplo de cuestionario</t>
+  </si>
+  <si>
+    <t>1.2 Ejemplo de cuestionario</t>
+  </si>
+  <si>
+    <t>1.1 Ejemplo de libro de códigos</t>
+  </si>
+  <si>
+    <t>1.2 Ejemplo de libro de códigos</t>
+  </si>
+  <si>
+    <t>1.1 Ejemplo de ficha técnica</t>
+  </si>
+  <si>
+    <t>1.2 Ejemplo de ficha técnica</t>
   </si>
 </sst>
 </file>
@@ -520,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D96ED4-54E1-4EA5-B33D-A1FCA11A3BB3}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,7 +606,7 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -611,7 +623,7 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -628,7 +640,7 @@
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -645,7 +657,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -662,7 +674,7 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -679,7 +691,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -696,7 +708,7 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -713,7 +725,7 @@
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -730,7 +742,7 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -747,7 +759,7 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -929,12 +941,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E13"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
@@ -944,6 +950,12 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>